<commit_message>
update dashboard + attendance logic
</commit_message>
<xml_diff>
--- a/mfc_socios_to_import_FINAL16.xlsx
+++ b/mfc_socios_to_import_FINAL16.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WR\madrugadores-app\carpeta 2\madrugadores-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1457C105-72C8-4A9A-A7B0-6D9BFA6BD1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D837D604-AA4D-4EF3-82BD-AE14FA6E9015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4B8E8B8B-0AE4-4119-86C5-82C0B08C49EF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>full_name</t>
   </si>
@@ -60,13 +60,22 @@
     <t>socio</t>
   </si>
   <si>
-    <t>rubenzhito94@gmail.com</t>
-  </si>
-  <si>
     <t>Luis Enrique Reinoso Valentín</t>
   </si>
   <si>
     <t>Velez Sarsfield</t>
+  </si>
+  <si>
+    <t>luisreinoso.03@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rubenzhito94@gmail.com </t>
+  </si>
+  <si>
+    <t>San Lorenzo</t>
+  </si>
+  <si>
+    <t>RUVERLI TENAZOA ONORBE</t>
   </si>
 </sst>
 </file>
@@ -460,7 +469,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,23 +500,37 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>45491362</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>73789548</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
@@ -536,8 +559,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{D911A838-25F6-49E3-BF2E-43EA809CDFB1}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{775C56D0-4DB7-44F3-8F82-89B7451BBBEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix RLS training_fines insert + session debug + Peru timezone fix
</commit_message>
<xml_diff>
--- a/mfc_socios_to_import_FINAL16.xlsx
+++ b/mfc_socios_to_import_FINAL16.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WR\madrugadores-app\carpeta 2\madrugadores-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D837D604-AA4D-4EF3-82BD-AE14FA6E9015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A481DFB-4CC1-45DC-B134-68D8AAC61196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4B8E8B8B-0AE4-4119-86C5-82C0B08C49EF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>full_name</t>
   </si>
@@ -60,22 +60,13 @@
     <t>socio</t>
   </si>
   <si>
-    <t>Luis Enrique Reinoso Valentín</t>
-  </si>
-  <si>
-    <t>Velez Sarsfield</t>
-  </si>
-  <si>
-    <t>luisreinoso.03@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rubenzhito94@gmail.com </t>
-  </si>
-  <si>
-    <t>San Lorenzo</t>
-  </si>
-  <si>
-    <t>RUVERLI TENAZOA ONORBE</t>
+    <t>Racing</t>
+  </si>
+  <si>
+    <t>tafur.fredy@gmail.com</t>
+  </si>
+  <si>
+    <t>Fredy Tafur Garay</t>
   </si>
 </sst>
 </file>
@@ -469,7 +460,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,37 +491,23 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>41863284</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>45491362</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>73789548</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
@@ -557,11 +534,7 @@
       <c r="B16" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{D911A838-25F6-49E3-BF2E-43EA809CDFB1}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{775C56D0-4DB7-44F3-8F82-89B7451BBBEF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>